<commit_message>
new round for ekstraklasa
</commit_message>
<xml_diff>
--- a/matchRoundEkstraklasa.xlsx
+++ b/matchRoundEkstraklasa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Typer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E4EEDD9D-F4E0-46D3-82FE-8957F182A58C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EF7026F-9109-4CC8-851D-B36FDD687BB6}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20736" windowHeight="8698" xr2:uid="{08337BA2-47F5-4B03-A043-CE74ED2B7BE1}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>name</t>
   </si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t>kolejka 11</t>
+  </si>
+  <si>
+    <t>kolejka 12</t>
   </si>
 </sst>
 </file>
@@ -391,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6D1B7A5-33BB-485A-A0AE-5D23F6E0D72F}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -418,6 +421,14 @@
         <v>4</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>